<commit_message>
Add 95% HPD intervals to table with tree heights and clock rates
</commit_message>
<xml_diff>
--- a/Tables/Tree_heights_and_clock_rates.xlsx
+++ b/Tables/Tree_heights_and_clock_rates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mate_\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mate_\Downloads\Diploma\virus-recombination\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B910092-5187-4DDA-8F44-1FC7E74E374D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F91840-D795-4209-916C-6FA0647D01F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96AAC1F1-33EA-4139-ABAB-1DF4CE06DC06}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Serotype</t>
   </si>
@@ -55,6 +55,72 @@
   </si>
   <si>
     <t>SAT1</t>
+  </si>
+  <si>
+    <t>[1405.7829, 1681.2922]</t>
+  </si>
+  <si>
+    <t>[84.7865, 244.5014]</t>
+  </si>
+  <si>
+    <t>Tree.height 95% HPD interval</t>
+  </si>
+  <si>
+    <t>clockRate/ucldMean 95% HPD interval</t>
+  </si>
+  <si>
+    <t>[1.7678E-3, 4.4727E-3]</t>
+  </si>
+  <si>
+    <t>[2.246E-3, 5.1772E-3]</t>
+  </si>
+  <si>
+    <t>[81.2028, 207.3966]</t>
+  </si>
+  <si>
+    <t>[1E-4, 1.1481E-4]</t>
+  </si>
+  <si>
+    <t>[1443.9537, 1695.5336]</t>
+  </si>
+  <si>
+    <t>[1E-4, 1.12E-4]</t>
+  </si>
+  <si>
+    <t>[1362.3057, 1703.4225]</t>
+  </si>
+  <si>
+    <t>[1E-4, 1.1832E-4]</t>
+  </si>
+  <si>
+    <t>[97.5098, 196.6163]</t>
+  </si>
+  <si>
+    <t>[1.2092E-3, 2.8237E-3]</t>
+  </si>
+  <si>
+    <t>[94.9937, 189.1976]</t>
+  </si>
+  <si>
+    <t>[1.1492E-3, 2.6736E-3]</t>
+  </si>
+  <si>
+    <t>[87.8278, 178.9122]</t>
+  </si>
+  <si>
+    <t>[97.33, 176.8925]</t>
+  </si>
+  <si>
+    <t>[1.4176E-3, 2.832E-3]</t>
+  </si>
+  <si>
+    <t>[1.2081E-3, 2.947E-3]</t>
+  </si>
+  <si>
+    <t>[108.1109, 618.647]</t>
+  </si>
+  <si>
+    <t>[9.6834E-4, 2.6446E-3]</t>
   </si>
 </sst>
 </file>
@@ -91,8 +157,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -407,19 +476,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E18393-A2C5-4C49-961B-BC8EFFD3916B}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="50.28515625" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,105 +500,163 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C2">
-        <v>2.5500000000000002E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.0300000000000001E-3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="C3">
-        <v>2.5409999999999999E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
       <c r="B4">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C4">
-        <v>2.643E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
+        <v>1.9810000000000001E-3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C5">
-        <v>1.9810000000000001E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.892E-3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C6">
-        <v>1.892E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.0579999999999999E-3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C7">
-        <v>2.0579999999999999E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.0699999999999998E-3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
       <c r="B8">
-        <v>134</v>
+        <v>1554</v>
       </c>
       <c r="C8">
-        <v>2.0699999999999998E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
+        <v>1.56E-4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>1554</v>
+        <v>1579</v>
       </c>
       <c r="C9">
-        <v>1.56E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.041E-4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1545</v>
       </c>
       <c r="C10">
         <v>1.0670000000000001E-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
       <c r="B11">
-        <v>1579</v>
+        <v>208</v>
       </c>
       <c r="C11">
-        <v>1.041E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12">
-        <v>208</v>
-      </c>
-      <c r="C12">
         <v>1.738E-3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add fixed O sample BEAST trees
</commit_message>
<xml_diff>
--- a/Tables/Tree_heights_and_clock_rates.xlsx
+++ b/Tables/Tree_heights_and_clock_rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mate_\Downloads\Diploma\virus-recombination\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F91840-D795-4209-916C-6FA0647D01F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847973A0-79FE-40BE-AAF2-45B70BFD04C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{96AAC1F1-33EA-4139-ABAB-1DF4CE06DC06}"/>
+    <workbookView xWindow="-6795" yWindow="4845" windowWidth="15765" windowHeight="12990" xr2:uid="{96AAC1F1-33EA-4139-ABAB-1DF4CE06DC06}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Serotype</t>
   </si>
@@ -93,34 +93,46 @@
     <t>[1E-4, 1.1832E-4]</t>
   </si>
   <si>
-    <t>[97.5098, 196.6163]</t>
-  </si>
-  <si>
-    <t>[1.2092E-3, 2.8237E-3]</t>
-  </si>
-  <si>
-    <t>[94.9937, 189.1976]</t>
-  </si>
-  <si>
-    <t>[1.1492E-3, 2.6736E-3]</t>
-  </si>
-  <si>
-    <t>[87.8278, 178.9122]</t>
-  </si>
-  <si>
-    <t>[97.33, 176.8925]</t>
-  </si>
-  <si>
-    <t>[1.4176E-3, 2.832E-3]</t>
-  </si>
-  <si>
-    <t>[1.2081E-3, 2.947E-3]</t>
-  </si>
-  <si>
     <t>[108.1109, 618.647]</t>
   </si>
   <si>
     <t>[9.6834E-4, 2.6446E-3]</t>
+  </si>
+  <si>
+    <t>2.427E-3</t>
+  </si>
+  <si>
+    <t>[102.2586, 217.8057]</t>
+  </si>
+  <si>
+    <t>[1.7203E-3, 3.2179E-3]</t>
+  </si>
+  <si>
+    <t>2.646E-3</t>
+  </si>
+  <si>
+    <t>[92.2312, 195.4317]</t>
+  </si>
+  <si>
+    <t>[1.8441E-3, 3.4851E-3]</t>
+  </si>
+  <si>
+    <t>3.131E-3</t>
+  </si>
+  <si>
+    <t>[2.4521E-3, 3.8491E-3]</t>
+  </si>
+  <si>
+    <t>[82.6899, 126.053]</t>
+  </si>
+  <si>
+    <t>2.664E-3</t>
+  </si>
+  <si>
+    <t>[96.3805, 197.7668]</t>
+  </si>
+  <si>
+    <t>[1.8559E-3, 3.4921E-3]</t>
   </si>
 </sst>
 </file>
@@ -479,13 +491,13 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="50.28515625" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" customWidth="1"/>
     <col min="5" max="5" width="35.7109375" customWidth="1"/>
   </cols>
@@ -543,58 +555,58 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>143</v>
-      </c>
-      <c r="C4">
-        <v>1.9810000000000001E-3</v>
+        <v>154</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>138</v>
-      </c>
-      <c r="C5">
-        <v>1.892E-3</v>
+        <v>140</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>130</v>
-      </c>
-      <c r="C6">
-        <v>2.0579999999999999E-3</v>
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>134</v>
-      </c>
-      <c r="C7">
-        <v>2.0699999999999998E-3</v>
+        <v>142</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -653,10 +665,10 @@
         <v>1.738E-3</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>